<commit_message>
Se modifica employee_turnover.xlsx y se actualiza survey_analysis.ipynb
</commit_message>
<xml_diff>
--- a/data/raw/employee_turnover.xlsx
+++ b/data/raw/employee_turnover.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E083318-E052-491E-B6CF-E4F0C3AE0222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E392BB-38DD-443D-B2F7-33FFA0D06DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="59">
   <si>
     <t>andres.reyes@inscomexico.com</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>tiempo_empresa</t>
+  </si>
+  <si>
+    <t>Metrologo Jr.</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K25"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +623,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>41</v>
@@ -725,7 +728,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>41</v>
@@ -795,7 +798,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>41</v>
@@ -830,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>41</v>
@@ -865,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>41</v>
@@ -935,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>41</v>
@@ -1005,7 +1008,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>41</v>
@@ -1040,7 +1043,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>41</v>
@@ -1128,7 +1131,7 @@
         <v>5</v>
       </c>
       <c r="I16">
-        <v>228000</v>
+        <v>108000</v>
       </c>
       <c r="J16">
         <v>24</v>
@@ -1180,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>41</v>
@@ -1390,7 +1393,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
@@ -1425,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>41</v>

</xml_diff>